<commit_message>
--- Deleted lib files --- Deleted tests files *** modified docs
</commit_message>
<xml_diff>
--- a/doc/AlterNative DOCS/Features supported.xlsx
+++ b/doc/AlterNative DOCS/Features supported.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\AlterNative\doc\AlterNative DOCS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="28515" windowHeight="12585"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Basic Statements</t>
   </si>
@@ -76,13 +81,16 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Constraints</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +145,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -183,7 +199,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -215,9 +231,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -249,6 +266,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -424,21 +442,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C8:E24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C8:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="33.140625" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="3:5">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>1</v>
       </c>
@@ -449,7 +467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="3:5">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>0</v>
       </c>
@@ -457,7 +475,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="3:5">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>4</v>
       </c>
@@ -465,7 +483,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="3:5">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>5</v>
       </c>
@@ -473,7 +491,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="3:5">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>6</v>
       </c>
@@ -481,7 +499,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="3:5">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>7</v>
       </c>
@@ -489,7 +507,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="3:5">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>8</v>
       </c>
@@ -497,7 +515,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="3:5">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>9</v>
       </c>
@@ -505,7 +523,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="3:5">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>10</v>
       </c>
@@ -513,7 +531,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="3:5">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>11</v>
       </c>
@@ -521,7 +539,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="3:5">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>12</v>
       </c>
@@ -529,7 +547,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="3:5" ht="14.25" customHeight="1">
+    <row r="20" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>13</v>
       </c>
@@ -537,7 +555,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="3:5" ht="14.25" customHeight="1">
+    <row r="21" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>15</v>
       </c>
@@ -545,7 +563,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="3:5">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>14</v>
       </c>
@@ -553,7 +571,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="3:5">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>16</v>
       </c>
@@ -561,7 +579,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="3:5">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>17</v>
       </c>
@@ -569,13 +587,21 @@
         <v>19</v>
       </c>
     </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E10:E24">
+  <conditionalFormatting sqref="E10:E25">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -588,24 +614,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
*** AlterNative.Core merged with AlterNative files
</commit_message>
<xml_diff>
--- a/doc/AlterNative DOCS/Features supported.xlsx
+++ b/doc/AlterNative DOCS/Features supported.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Basic Statements</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Constraints</t>
+  </si>
+  <si>
+    <t>Delegates</t>
   </si>
 </sst>
 </file>
@@ -443,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C8:E25"/>
+  <dimension ref="C8:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,8 +598,16 @@
         <v>18</v>
       </c>
     </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E10:E25">
+  <conditionalFormatting sqref="E10:E26">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>